<commit_message>
fasta file with many strings
</commit_message>
<xml_diff>
--- a/container/src/static/data/all_sequences.xlsx
+++ b/container/src/static/data/all_sequences.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Maria\Maria_scripts\HDR_flask\container\src\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Maria\Maria_scripts\HDR_flask\container\src\static\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="194">
   <si>
     <t>Elements</t>
   </si>
@@ -582,13 +582,37 @@
   </si>
   <si>
     <t>The woodchuck hepatitis virus post-transcriptional regulatory element</t>
+  </si>
+  <si>
+    <t>GGAAGCGGAgagggcagaggcagtctgctgacatgcggtgacgtggaagagaatcccggccct</t>
+  </si>
+  <si>
+    <t>GGAAGCGGAgccaccaacttctccctgctgaagcaggccggcgacgtggaggagaaccccggcccc</t>
+  </si>
+  <si>
+    <t>GGAAGCGGAcagtgtactaattatgctctcttgaaattggctggagatgttgagagcaacccaggtccc</t>
+  </si>
+  <si>
+    <t>GGAAGCGGAgtgaaacagactttgaattttgaccttctcaagttggcgggagacgtggagtccaaccctggacct</t>
+  </si>
+  <si>
+    <t>GSG-T2A</t>
+  </si>
+  <si>
+    <t>GSG-P2A</t>
+  </si>
+  <si>
+    <t>GSG-E2A</t>
+  </si>
+  <si>
+    <t>GSG-F2A</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -615,6 +639,12 @@
       <name val="Candara"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -636,7 +666,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -650,6 +680,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -931,10 +967,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E75"/>
+  <dimension ref="A1:E79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection sqref="A1:E1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="C81" sqref="C81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2103,6 +2139,62 @@
         <v>1</v>
       </c>
     </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A76" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B76" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="C76" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="E76" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A77" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B77" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="C77" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="E77" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A78" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B78" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="C78" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="E78" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A79" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B79" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="C79" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="E79" s="7">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:E75">
     <sortCondition ref="A1"/>

</xml_diff>